<commit_message>
idk measurements and stuff
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gadibessudo/Library/CloudStorage/GoogleDrive-gadibessudo@gmail.com/My Drive/Projects/University/Lab C/2025a/PaulTrap/paul-trap-experiment-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D1DC17F-B735-A047-82E5-46EF6C191F64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A11A420-4EE5-0649-B9CA-9A27C6290CCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38400" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="0_raw_laser" sheetId="1" r:id="rId1"/>
     <sheet name="1_filtered_data" sheetId="2" r:id="rId2"/>
+    <sheet name="2_stick_measurements" sheetId="3" r:id="rId3"/>
+    <sheet name="3_particle_measurements" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_Hlk182785910" localSheetId="0">'0_raw_laser'!$G$20</definedName>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="55">
   <si>
     <t>picture_name</t>
   </si>
@@ -163,6 +165,45 @@
   </si>
   <si>
     <t>height_error-pixels</t>
+  </si>
+  <si>
+    <t>DSC03209.JPG</t>
+  </si>
+  <si>
+    <t>DSC03210.JPG</t>
+  </si>
+  <si>
+    <t>DSC03211.JPG</t>
+  </si>
+  <si>
+    <t>DSC03212.JPG</t>
+  </si>
+  <si>
+    <t>DSC03213.JPG</t>
+  </si>
+  <si>
+    <t>DSC03214.JPG</t>
+  </si>
+  <si>
+    <t>diameter_length_error-pixels</t>
+  </si>
+  <si>
+    <t>diameter_length-pixels</t>
+  </si>
+  <si>
+    <t>diameter_measure_horizontal_diff</t>
+  </si>
+  <si>
+    <t>diameter_measure_vertical_diff</t>
+  </si>
+  <si>
+    <t>DSC03162.JPG</t>
+  </si>
+  <si>
+    <t>DSC03163.JPG</t>
+  </si>
+  <si>
+    <t>diameter-pixels</t>
   </si>
 </sst>
 </file>
@@ -534,8 +575,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2660,4 +2701,219 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5AF7B89-D012-724A-AEBE-8F94F0049580}">
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2">
+        <v>2105</v>
+      </c>
+      <c r="D2">
+        <v>131</v>
+      </c>
+      <c r="E2">
+        <f>SQRT(C2^2+D2^2)</f>
+        <v>2109.0723079117038</v>
+      </c>
+      <c r="F2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3">
+        <v>2112</v>
+      </c>
+      <c r="D3">
+        <v>111</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E7" si="0">SQRT(C3^2+D3^2)</f>
+        <v>2114.9148919046365</v>
+      </c>
+      <c r="F3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4">
+        <v>2112</v>
+      </c>
+      <c r="D4">
+        <v>48</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>2112.5453841278772</v>
+      </c>
+      <c r="F4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5">
+        <v>2099</v>
+      </c>
+      <c r="D5">
+        <v>84</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>2100.680127958562</v>
+      </c>
+      <c r="F5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6">
+        <v>2093</v>
+      </c>
+      <c r="D6">
+        <v>36</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>2093.3095805446455</v>
+      </c>
+      <c r="F6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7">
+        <v>2106</v>
+      </c>
+      <c r="D7">
+        <v>71</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>2107.1964787366173</v>
+      </c>
+      <c r="F7">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3BDE8B2-30EC-904D-BBDC-B27B4B26C860}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
renamed dc volts to kilovolts
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gadibessudo/Library/CloudStorage/GoogleDrive-gadibessudo@gmail.com/My Drive/Projects/University/Lab C/2025a/PaulTrap/paul-trap-experiment-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EFD38A7-5CB6-E640-BE5F-7A274C2880D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79B19D6B-1AD8-9E46-9952-CB1AF2AEC063}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38420" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20" yWindow="300" windowWidth="30240" windowHeight="19340" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="0_raw_laser" sheetId="1" r:id="rId1"/>
@@ -150,12 +150,6 @@
     <t>top_pixel_error</t>
   </si>
   <si>
-    <t>DC-volts</t>
-  </si>
-  <si>
-    <t>DC_error-volts</t>
-  </si>
-  <si>
     <t>length-pixels</t>
   </si>
   <si>
@@ -216,7 +210,13 @@
     <t>DSC03208.JPG</t>
   </si>
   <si>
-    <t>dc-volts</t>
+    <t>DC-kilovolts</t>
+  </si>
+  <si>
+    <t>DC_error-kilovolts</t>
+  </si>
+  <si>
+    <t>dc-kilovolts</t>
   </si>
 </sst>
 </file>
@@ -589,7 +589,7 @@
   <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D6"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -614,10 +614,10 @@
         <v>35</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -1437,7 +1437,7 @@
   <dimension ref="A1:L30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1474,22 +1474,22 @@
         <v>35</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
@@ -2731,16 +2731,16 @@
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -2748,7 +2748,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C2">
         <v>2105</v>
@@ -2769,7 +2769,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C3">
         <v>2112</v>
@@ -2790,7 +2790,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C4">
         <v>2112</v>
@@ -2811,7 +2811,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C5">
         <v>2099</v>
@@ -2832,7 +2832,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C6">
         <v>2093</v>
@@ -2853,7 +2853,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C7">
         <v>2106</v>
@@ -2890,7 +2890,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -2898,7 +2898,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C2">
         <v>48</v>
@@ -2909,7 +2909,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C3">
         <v>49</v>
@@ -2937,7 +2937,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2955,7 +2955,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C2">
         <v>0.67618999999999996</v>
@@ -2966,7 +2966,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C3">
         <v>0.67891999999999997</v>
@@ -2977,7 +2977,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C4">
         <v>0.67488000000000004</v>

</xml_diff>

<commit_message>
Tried fixing length and height calculation
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gadibessudo/Library/CloudStorage/GoogleDrive-gadibessudo@gmail.com/My Drive/Projects/University/Lab C/2025a/PaulTrap/paul-trap-experiment-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E625F910-9807-E042-881F-6466905FB25A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A08FE1E2-11C8-4241-8791-3453145CE1F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="300" windowWidth="30240" windowHeight="19340" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4080" yWindow="1380" windowWidth="30240" windowHeight="19340" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="0_raw_laser" sheetId="1" r:id="rId1"/>
@@ -1437,7 +1437,7 @@
   <dimension ref="A1:L30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="M32" sqref="M32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1518,16 +1518,16 @@
         <v>1E-4</v>
       </c>
       <c r="I2" s="3">
-        <f>C2-E2</f>
-        <v>76</v>
+        <f>C2-E2-76</f>
+        <v>0</v>
       </c>
       <c r="J2" s="3">
         <f>SQRT(D2^2+F2^2)</f>
         <v>21.213203435596427</v>
       </c>
       <c r="K2" s="3">
-        <f>(C2+E2)/2</f>
-        <v>1614</v>
+        <f>1614-(C2+E2)/2</f>
+        <v>0</v>
       </c>
       <c r="L2" s="3">
         <f>SQRT(D2^2+F2^2)</f>
@@ -1560,16 +1560,16 @@
         <v>1E-4</v>
       </c>
       <c r="I3" s="3">
-        <f t="shared" ref="I3:I20" si="0">C3-E3</f>
-        <v>117</v>
+        <f t="shared" ref="I3:I20" si="0">C3-E3-76</f>
+        <v>41</v>
       </c>
       <c r="J3" s="3">
         <f t="shared" ref="J3:J30" si="1">SQRT(D3^2+F3^2)</f>
         <v>21.213203435596427</v>
       </c>
       <c r="K3" s="3">
-        <f t="shared" ref="K3:K20" si="2">(C3+E3)/2</f>
-        <v>1576.5</v>
+        <f t="shared" ref="K3:K30" si="2">1614-(C3+E3)/2</f>
+        <v>37.5</v>
       </c>
       <c r="L3" s="3">
         <f t="shared" ref="L3:L30" si="3">SQRT(D3^2+F3^2)</f>
@@ -1603,7 +1603,7 @@
       </c>
       <c r="I4" s="3">
         <f t="shared" si="0"/>
-        <v>165</v>
+        <v>89</v>
       </c>
       <c r="J4" s="3">
         <f t="shared" si="1"/>
@@ -1611,7 +1611,7 @@
       </c>
       <c r="K4" s="3">
         <f t="shared" si="2"/>
-        <v>1548.5</v>
+        <v>65.5</v>
       </c>
       <c r="L4" s="3">
         <f t="shared" si="3"/>
@@ -1645,7 +1645,7 @@
       </c>
       <c r="I5" s="3">
         <f t="shared" si="0"/>
-        <v>224</v>
+        <v>148</v>
       </c>
       <c r="J5" s="3">
         <f t="shared" si="1"/>
@@ -1653,7 +1653,7 @@
       </c>
       <c r="K5" s="3">
         <f t="shared" si="2"/>
-        <v>1516</v>
+        <v>98</v>
       </c>
       <c r="L5" s="3">
         <f t="shared" si="3"/>
@@ -1687,7 +1687,7 @@
       </c>
       <c r="I6" s="3">
         <f t="shared" si="0"/>
-        <v>276</v>
+        <v>200</v>
       </c>
       <c r="J6" s="3">
         <f t="shared" si="1"/>
@@ -1695,7 +1695,7 @@
       </c>
       <c r="K6" s="3">
         <f t="shared" si="2"/>
-        <v>1484</v>
+        <v>130</v>
       </c>
       <c r="L6" s="3">
         <f t="shared" si="3"/>
@@ -1729,7 +1729,7 @@
       </c>
       <c r="I7" s="3">
         <f t="shared" si="0"/>
-        <v>332</v>
+        <v>256</v>
       </c>
       <c r="J7" s="3">
         <f t="shared" si="1"/>
@@ -1737,7 +1737,7 @@
       </c>
       <c r="K7" s="3">
         <f t="shared" si="2"/>
-        <v>1451</v>
+        <v>163</v>
       </c>
       <c r="L7" s="3">
         <f t="shared" si="3"/>
@@ -1771,7 +1771,7 @@
       </c>
       <c r="I8" s="3">
         <f t="shared" si="0"/>
-        <v>390</v>
+        <v>314</v>
       </c>
       <c r="J8" s="3">
         <f t="shared" si="1"/>
@@ -1779,7 +1779,7 @@
       </c>
       <c r="K8" s="3">
         <f t="shared" si="2"/>
-        <v>1416</v>
+        <v>198</v>
       </c>
       <c r="L8" s="3">
         <f t="shared" si="3"/>
@@ -1813,7 +1813,7 @@
       </c>
       <c r="I9" s="3">
         <f t="shared" si="0"/>
-        <v>466</v>
+        <v>390</v>
       </c>
       <c r="J9" s="3">
         <f t="shared" si="1"/>
@@ -1821,7 +1821,7 @@
       </c>
       <c r="K9" s="3">
         <f t="shared" si="2"/>
-        <v>1377</v>
+        <v>237</v>
       </c>
       <c r="L9" s="3">
         <f t="shared" si="3"/>
@@ -1855,7 +1855,7 @@
       </c>
       <c r="I10" s="3">
         <f t="shared" si="0"/>
-        <v>515</v>
+        <v>439</v>
       </c>
       <c r="J10" s="3">
         <f t="shared" si="1"/>
@@ -1863,7 +1863,7 @@
       </c>
       <c r="K10" s="3">
         <f t="shared" si="2"/>
-        <v>1346.5</v>
+        <v>267.5</v>
       </c>
       <c r="L10" s="3">
         <f t="shared" si="3"/>
@@ -1897,7 +1897,7 @@
       </c>
       <c r="I11" s="3">
         <f t="shared" si="0"/>
-        <v>580</v>
+        <v>504</v>
       </c>
       <c r="J11" s="3">
         <f t="shared" si="1"/>
@@ -1905,7 +1905,7 @@
       </c>
       <c r="K11" s="3">
         <f t="shared" si="2"/>
-        <v>1307</v>
+        <v>307</v>
       </c>
       <c r="L11" s="3">
         <f t="shared" si="3"/>
@@ -1939,7 +1939,7 @@
       </c>
       <c r="I12" s="3">
         <f t="shared" si="0"/>
-        <v>638</v>
+        <v>562</v>
       </c>
       <c r="J12" s="3">
         <f t="shared" si="1"/>
@@ -1947,7 +1947,7 @@
       </c>
       <c r="K12" s="3">
         <f t="shared" si="2"/>
-        <v>1276</v>
+        <v>338</v>
       </c>
       <c r="L12" s="3">
         <f t="shared" si="3"/>
@@ -1981,7 +1981,7 @@
       </c>
       <c r="I13" s="3">
         <f t="shared" si="0"/>
-        <v>695</v>
+        <v>619</v>
       </c>
       <c r="J13" s="3">
         <f t="shared" si="1"/>
@@ -1989,7 +1989,7 @@
       </c>
       <c r="K13" s="3">
         <f t="shared" si="2"/>
-        <v>1245.5</v>
+        <v>368.5</v>
       </c>
       <c r="L13" s="3">
         <f t="shared" si="3"/>
@@ -2023,7 +2023,7 @@
       </c>
       <c r="I14" s="3">
         <f t="shared" si="0"/>
-        <v>752</v>
+        <v>676</v>
       </c>
       <c r="J14" s="3">
         <f t="shared" si="1"/>
@@ -2031,7 +2031,7 @@
       </c>
       <c r="K14" s="3">
         <f t="shared" si="2"/>
-        <v>1216</v>
+        <v>398</v>
       </c>
       <c r="L14" s="3">
         <f t="shared" si="3"/>
@@ -2065,7 +2065,7 @@
       </c>
       <c r="I15" s="3">
         <f t="shared" si="0"/>
-        <v>809</v>
+        <v>733</v>
       </c>
       <c r="J15" s="3">
         <f t="shared" si="1"/>
@@ -2073,7 +2073,7 @@
       </c>
       <c r="K15" s="3">
         <f t="shared" si="2"/>
-        <v>1178.5</v>
+        <v>435.5</v>
       </c>
       <c r="L15" s="3">
         <f t="shared" si="3"/>
@@ -2107,7 +2107,7 @@
       </c>
       <c r="I16" s="3">
         <f t="shared" si="0"/>
-        <v>874</v>
+        <v>798</v>
       </c>
       <c r="J16" s="3">
         <f t="shared" si="1"/>
@@ -2115,7 +2115,7 @@
       </c>
       <c r="K16" s="3">
         <f t="shared" si="2"/>
-        <v>1140</v>
+        <v>474</v>
       </c>
       <c r="L16" s="3">
         <f t="shared" si="3"/>
@@ -2149,7 +2149,7 @@
       </c>
       <c r="I17" s="3">
         <f t="shared" si="0"/>
-        <v>981</v>
+        <v>905</v>
       </c>
       <c r="J17" s="3">
         <f t="shared" si="1"/>
@@ -2157,7 +2157,7 @@
       </c>
       <c r="K17" s="3">
         <f t="shared" si="2"/>
-        <v>1083.5</v>
+        <v>530.5</v>
       </c>
       <c r="L17" s="3">
         <f t="shared" si="3"/>
@@ -2191,7 +2191,7 @@
       </c>
       <c r="I18" s="3">
         <f t="shared" si="0"/>
-        <v>1037</v>
+        <v>961</v>
       </c>
       <c r="J18" s="3">
         <f t="shared" si="1"/>
@@ -2199,7 +2199,7 @@
       </c>
       <c r="K18" s="3">
         <f t="shared" si="2"/>
-        <v>1056.5</v>
+        <v>557.5</v>
       </c>
       <c r="L18" s="3">
         <f t="shared" si="3"/>
@@ -2233,7 +2233,7 @@
       </c>
       <c r="I19" s="3">
         <f t="shared" si="0"/>
-        <v>1108</v>
+        <v>1032</v>
       </c>
       <c r="J19" s="3">
         <f t="shared" si="1"/>
@@ -2241,7 +2241,7 @@
       </c>
       <c r="K19" s="3">
         <f t="shared" si="2"/>
-        <v>1025</v>
+        <v>589</v>
       </c>
       <c r="L19" s="3">
         <f t="shared" si="3"/>
@@ -2275,7 +2275,7 @@
       </c>
       <c r="I20" s="3">
         <f t="shared" si="0"/>
-        <v>1054</v>
+        <v>978</v>
       </c>
       <c r="J20" s="3">
         <f t="shared" si="1"/>
@@ -2283,7 +2283,7 @@
       </c>
       <c r="K20" s="3">
         <f t="shared" si="2"/>
-        <v>1043</v>
+        <v>571</v>
       </c>
       <c r="L20" s="3">
         <f t="shared" si="3"/>
@@ -2316,16 +2316,16 @@
         <v>1E-4</v>
       </c>
       <c r="I21" s="3">
-        <f>E21-C21</f>
-        <v>-116</v>
+        <f>E21-C21+76</f>
+        <v>-40</v>
       </c>
       <c r="J21" s="3">
         <f t="shared" si="1"/>
         <v>21.213203435596427</v>
       </c>
       <c r="K21" s="3">
-        <f>(C21+E21)/2</f>
-        <v>1646</v>
+        <f t="shared" si="2"/>
+        <v>-32</v>
       </c>
       <c r="L21" s="3">
         <f t="shared" si="3"/>
@@ -2358,16 +2358,16 @@
         <v>1E-4</v>
       </c>
       <c r="I22" s="3">
-        <f t="shared" ref="I22:I30" si="4">E22-C22</f>
-        <v>-168</v>
+        <f t="shared" ref="I22:I30" si="4">E22-C22+76</f>
+        <v>-92</v>
       </c>
       <c r="J22" s="3">
         <f t="shared" si="1"/>
         <v>21.213203435596427</v>
       </c>
       <c r="K22" s="3">
-        <f t="shared" ref="K22:K30" si="5">(C22+E22)/2</f>
-        <v>1684</v>
+        <f t="shared" si="2"/>
+        <v>-70</v>
       </c>
       <c r="L22" s="3">
         <f t="shared" si="3"/>
@@ -2401,15 +2401,15 @@
       </c>
       <c r="I23" s="3">
         <f t="shared" si="4"/>
-        <v>-296</v>
+        <v>-220</v>
       </c>
       <c r="J23" s="3">
         <f t="shared" si="1"/>
         <v>21.213203435596427</v>
       </c>
       <c r="K23" s="3">
-        <f t="shared" si="5"/>
-        <v>1751</v>
+        <f t="shared" si="2"/>
+        <v>-137</v>
       </c>
       <c r="L23" s="3">
         <f t="shared" si="3"/>
@@ -2443,15 +2443,15 @@
       </c>
       <c r="I24" s="3">
         <f t="shared" si="4"/>
-        <v>-424</v>
+        <v>-348</v>
       </c>
       <c r="J24" s="3">
         <f t="shared" si="1"/>
         <v>21.213203435596427</v>
       </c>
       <c r="K24" s="3">
-        <f t="shared" si="5"/>
-        <v>1822</v>
+        <f t="shared" si="2"/>
+        <v>-208</v>
       </c>
       <c r="L24" s="3">
         <f t="shared" si="3"/>
@@ -2485,15 +2485,15 @@
       </c>
       <c r="I25" s="3">
         <f t="shared" si="4"/>
-        <v>-474</v>
+        <v>-398</v>
       </c>
       <c r="J25" s="3">
         <f t="shared" si="1"/>
         <v>21.213203435596427</v>
       </c>
       <c r="K25" s="3">
-        <f t="shared" si="5"/>
-        <v>1854</v>
+        <f t="shared" si="2"/>
+        <v>-240</v>
       </c>
       <c r="L25" s="3">
         <f t="shared" si="3"/>
@@ -2527,15 +2527,15 @@
       </c>
       <c r="I26" s="3">
         <f t="shared" si="4"/>
-        <v>-537</v>
+        <v>-461</v>
       </c>
       <c r="J26" s="3">
         <f t="shared" si="1"/>
         <v>21.213203435596427</v>
       </c>
       <c r="K26" s="3">
-        <f t="shared" si="5"/>
-        <v>1889.5</v>
+        <f t="shared" si="2"/>
+        <v>-275.5</v>
       </c>
       <c r="L26" s="3">
         <f t="shared" si="3"/>
@@ -2569,15 +2569,15 @@
       </c>
       <c r="I27" s="3">
         <f t="shared" si="4"/>
-        <v>-591</v>
+        <v>-515</v>
       </c>
       <c r="J27" s="3">
         <f t="shared" si="1"/>
         <v>21.213203435596427</v>
       </c>
       <c r="K27" s="3">
-        <f t="shared" si="5"/>
-        <v>1922.5</v>
+        <f t="shared" si="2"/>
+        <v>-308.5</v>
       </c>
       <c r="L27" s="3">
         <f t="shared" si="3"/>
@@ -2611,15 +2611,15 @@
       </c>
       <c r="I28" s="3">
         <f t="shared" si="4"/>
-        <v>-662</v>
+        <v>-586</v>
       </c>
       <c r="J28" s="3">
         <f t="shared" si="1"/>
         <v>21.213203435596427</v>
       </c>
       <c r="K28" s="3">
-        <f t="shared" si="5"/>
-        <v>1958</v>
+        <f t="shared" si="2"/>
+        <v>-344</v>
       </c>
       <c r="L28" s="3">
         <f t="shared" si="3"/>
@@ -2653,15 +2653,15 @@
       </c>
       <c r="I29" s="3">
         <f t="shared" si="4"/>
-        <v>-732</v>
+        <v>-656</v>
       </c>
       <c r="J29" s="3">
         <f t="shared" si="1"/>
         <v>21.213203435596427</v>
       </c>
       <c r="K29" s="3">
-        <f t="shared" si="5"/>
-        <v>2000</v>
+        <f t="shared" si="2"/>
+        <v>-386</v>
       </c>
       <c r="L29" s="3">
         <f t="shared" si="3"/>
@@ -2695,15 +2695,15 @@
       </c>
       <c r="I30" s="3">
         <f t="shared" si="4"/>
-        <v>-765</v>
+        <v>-689</v>
       </c>
       <c r="J30" s="3">
         <f t="shared" si="1"/>
         <v>21.213203435596427</v>
       </c>
       <c r="K30" s="3">
-        <f t="shared" si="5"/>
-        <v>2017.5</v>
+        <f t="shared" si="2"/>
+        <v>-403.5</v>
       </c>
       <c r="L30" s="3">
         <f t="shared" si="3"/>

</xml_diff>